<commit_message>
Revised, caught a few errors
</commit_message>
<xml_diff>
--- a/Tables_Figures/output/table08_PROP_example_stimulus.xlsx
+++ b/Tables_Figures/output/table08_PROP_example_stimulus.xlsx
@@ -41,22 +41,22 @@
     <t>Unrelated</t>
   </si>
   <si>
-    <t>The jar near the sticky lid</t>
+    <t>The atlas by the detailed map</t>
   </si>
   <si>
-    <t>The jar near the sticky cookie</t>
+    <t>The atlas by the detailed globe</t>
   </si>
   <si>
-    <t>The jar near the sticky bagel</t>
+    <t>The atlas by the detailed journal</t>
   </si>
   <si>
-    <t>The jar near the sticky lids</t>
+    <t>The atlas by the detailed maps</t>
   </si>
   <si>
-    <t>The jar near the sticky cookies</t>
+    <t>The atlas by the detailed globes</t>
   </si>
   <si>
-    <t>The jar near the sticky bagels</t>
+    <t>The atlas by the detailed journals</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Adding another regression summary for ease of reading
</commit_message>
<xml_diff>
--- a/Tables_Figures/output/table08_PROP_example_stimulus.xlsx
+++ b/Tables_Figures/output/table08_PROP_example_stimulus.xlsx
@@ -41,22 +41,22 @@
     <t>Unrelated</t>
   </si>
   <si>
-    <t>The atlas by the detailed map</t>
+    <t>The jar near the sticky lid</t>
   </si>
   <si>
-    <t>The atlas by the detailed globe</t>
+    <t>The jar near the sticky cookie</t>
   </si>
   <si>
-    <t>The atlas by the detailed journal</t>
+    <t>The jar near the stale bagel</t>
   </si>
   <si>
-    <t>The atlas by the detailed maps</t>
+    <t>The jar near the sticky lids</t>
   </si>
   <si>
-    <t>The atlas by the detailed globes</t>
+    <t>The jar near the sticky cookies</t>
   </si>
   <si>
-    <t>The atlas by the detailed journals</t>
+    <t>The jar near the stale bagels</t>
   </si>
 </sst>
 </file>

</xml_diff>